<commit_message>
Results from July 21, 2020 07:14:56 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-21.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-21.xlsx
@@ -525,16 +525,16 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="C2" t="n">
-        <v>28240</v>
+        <v>28606</v>
       </c>
       <c r="D2" t="n">
-        <v>753</v>
+        <v>758</v>
       </c>
       <c r="E2" t="n">
-        <v>3254</v>
+        <v>3321</v>
       </c>
       <c r="F2" t="n">
         <v>95</v>
@@ -572,13 +572,13 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="C3" t="n">
-        <v>31316</v>
+        <v>31867</v>
       </c>
       <c r="D3" t="n">
-        <v>262</v>
+        <v>274</v>
       </c>
       <c r="E3" t="n">
         <v>464</v>
@@ -623,29 +623,29 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>218478</t>
+          <t>219030</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>18787</t>
+          <t>18800</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>33757</v>
+        <v>33634</v>
       </c>
       <c r="F4" t="n">
-        <v>5258</v>
+        <v>5090</v>
       </c>
       <c r="G4" t="n">
-        <v>30.1</v>
+        <v>30.09</v>
       </c>
       <c r="H4" t="n">
-        <v>30.49</v>
+        <v>30.47</v>
       </c>
       <c r="I4" t="b">
         <v>0</v>
@@ -654,10 +654,10 @@
         <v>1</v>
       </c>
       <c r="K4" t="n">
-        <v>112160</v>
+        <v>111790</v>
       </c>
       <c r="L4" t="n">
-        <v>17245</v>
+        <v>16704</v>
       </c>
       <c r="M4" t="n">
         <v>2049418</v>
@@ -729,22 +729,22 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>44031</v>
+        <v>44032</v>
       </c>
       <c r="C6" t="n">
-        <v>5305</v>
+        <v>5340</v>
       </c>
       <c r="D6" t="n">
         <v>53</v>
       </c>
       <c r="E6" t="n">
-        <v>290</v>
+        <v>295</v>
       </c>
       <c r="F6" t="n">
         <v>5</v>
       </c>
       <c r="G6" t="n">
-        <v>6.36</v>
+        <v>6.41</v>
       </c>
       <c r="H6" t="n">
         <v>9.800000000000001</v>
@@ -756,7 +756,7 @@
         <v>0</v>
       </c>
       <c r="K6" t="n">
-        <v>4563</v>
+        <v>4599</v>
       </c>
       <c r="L6" t="n">
         <v>51</v>
@@ -776,25 +776,25 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="C7" t="n">
-        <v>79754</v>
+        <v>81944</v>
       </c>
       <c r="D7" t="n">
-        <v>847</v>
+        <v>871</v>
       </c>
       <c r="E7" t="n">
-        <v>15478</v>
+        <v>15752</v>
       </c>
       <c r="F7" t="n">
-        <v>305</v>
+        <v>315</v>
       </c>
       <c r="G7" t="n">
-        <v>19.41</v>
+        <v>19.22</v>
       </c>
       <c r="H7" t="n">
-        <v>36.01</v>
+        <v>36.17</v>
       </c>
       <c r="I7" t="b">
         <v>1</v>
@@ -823,21 +823,21 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>34526</t>
+          <t>35012</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>247</t>
+          <t>251</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>855</t>
+          <t>870</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -876,25 +876,25 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="C9" t="n">
-        <v>23414</v>
+        <v>24060</v>
       </c>
       <c r="D9" t="n">
-        <v>671</v>
+        <v>674</v>
       </c>
       <c r="E9" t="n">
-        <v>2444</v>
+        <v>2012</v>
       </c>
       <c r="F9" t="n">
-        <v>26</v>
+        <v>92</v>
       </c>
       <c r="G9" t="n">
-        <v>15.53</v>
+        <v>12.71</v>
       </c>
       <c r="H9" t="n">
-        <v>4.19</v>
+        <v>14.63</v>
       </c>
       <c r="I9" t="b">
         <v>0</v>
@@ -903,10 +903,10 @@
         <v>1</v>
       </c>
       <c r="K9" t="n">
-        <v>15738</v>
+        <v>15831</v>
       </c>
       <c r="L9" t="n">
-        <v>625</v>
+        <v>628</v>
       </c>
       <c r="M9" t="n">
         <v>354112</v>
@@ -930,22 +930,22 @@
         <v>44033</v>
       </c>
       <c r="C10" t="n">
-        <v>33927</v>
+        <v>34655</v>
       </c>
       <c r="D10" t="n">
-        <v>363</v>
+        <v>374</v>
       </c>
       <c r="E10" t="n">
-        <v>7167</v>
+        <v>7364</v>
       </c>
       <c r="F10" t="n">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="G10" t="n">
-        <v>24.61</v>
+        <v>24.62</v>
       </c>
       <c r="H10" t="n">
-        <v>26.24</v>
+        <v>26.61</v>
       </c>
       <c r="I10" t="b">
         <v>0</v>
@@ -954,10 +954,10 @@
         <v>1</v>
       </c>
       <c r="K10" t="n">
-        <v>29119</v>
+        <v>29915</v>
       </c>
       <c r="L10" t="n">
-        <v>362</v>
+        <v>372</v>
       </c>
       <c r="M10" t="n">
         <v>460970</v>
@@ -978,16 +978,16 @@
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="C11" t="n">
-        <v>24135</v>
+        <v>24520</v>
       </c>
       <c r="D11" t="n">
-        <v>478</v>
+        <v>487</v>
       </c>
       <c r="E11" t="n">
-        <v>880</v>
+        <v>895</v>
       </c>
       <c r="F11" t="n">
         <v>18</v>
@@ -996,7 +996,7 @@
         <v>4.69</v>
       </c>
       <c r="H11" t="n">
-        <v>3.9</v>
+        <v>3.74</v>
       </c>
       <c r="I11" t="b">
         <v>0</v>
@@ -1005,10 +1005,10 @@
         <v>0</v>
       </c>
       <c r="K11" t="n">
-        <v>18776</v>
+        <v>19099</v>
       </c>
       <c r="L11" t="n">
-        <v>462</v>
+        <v>481</v>
       </c>
       <c r="M11" t="n">
         <v>166412</v>
@@ -1029,22 +1029,22 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="C12" t="n">
-        <v>78375</v>
+        <v>79371</v>
       </c>
       <c r="D12" t="n">
-        <v>2031</v>
+        <v>2048</v>
       </c>
       <c r="E12" t="n">
-        <v>12678</v>
+        <v>12922</v>
       </c>
       <c r="F12" t="n">
-        <v>479</v>
+        <v>483</v>
       </c>
       <c r="G12" t="n">
-        <v>16.18</v>
+        <v>16.28</v>
       </c>
       <c r="H12" t="n">
         <v>23.58</v>
@@ -1076,16 +1076,16 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="C13" t="n">
-        <v>17215</v>
+        <v>17517</v>
       </c>
       <c r="D13" t="n">
-        <v>578</v>
+        <v>588</v>
       </c>
       <c r="E13" t="n">
-        <v>311</v>
+        <v>317</v>
       </c>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="n">
@@ -1119,20 +1119,20 @@
         </is>
       </c>
       <c r="B14" s="2" t="n">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="C14" t="n">
-        <v>87035</v>
+        <v>89557</v>
       </c>
       <c r="D14" t="n">
-        <v>1309</v>
+        <v>1325</v>
       </c>
       <c r="E14" t="n">
-        <v>8590</v>
+        <v>8754</v>
       </c>
       <c r="F14" t="inlineStr"/>
       <c r="G14" t="n">
-        <v>19.92</v>
+        <v>19.74</v>
       </c>
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="b">
@@ -1142,7 +1142,7 @@
         <v>1</v>
       </c>
       <c r="K14" t="n">
-        <v>43119</v>
+        <v>44336</v>
       </c>
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="n">
@@ -1164,20 +1164,20 @@
         </is>
       </c>
       <c r="B15" s="2" t="n">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="C15" t="n">
-        <v>23584</v>
+        <v>24011</v>
       </c>
       <c r="D15" t="n">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="E15" t="n">
-        <v>2980</v>
+        <v>3041</v>
       </c>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="n">
-        <v>24.92</v>
+        <v>24.95</v>
       </c>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="b">
@@ -1187,7 +1187,7 @@
         <v>1</v>
       </c>
       <c r="K15" t="n">
-        <v>11960</v>
+        <v>12187</v>
       </c>
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="n">
@@ -1209,25 +1209,25 @@
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="C16" t="n">
-        <v>67711</v>
+        <v>69075</v>
       </c>
       <c r="D16" t="n">
-        <v>1257</v>
+        <v>1268</v>
       </c>
       <c r="E16" t="n">
-        <v>20170</v>
+        <v>20540</v>
       </c>
       <c r="F16" t="n">
-        <v>538</v>
+        <v>542</v>
       </c>
       <c r="G16" t="n">
-        <v>43.85</v>
+        <v>43.75</v>
       </c>
       <c r="H16" t="n">
-        <v>44.68</v>
+        <v>44.65</v>
       </c>
       <c r="I16" t="b">
         <v>0</v>
@@ -1236,10 +1236,10 @@
         <v>0</v>
       </c>
       <c r="K16" t="n">
-        <v>45993</v>
+        <v>46948</v>
       </c>
       <c r="L16" t="n">
-        <v>1204</v>
+        <v>1214</v>
       </c>
       <c r="M16" t="n">
         <v>1293186</v>
@@ -1260,25 +1260,25 @@
         </is>
       </c>
       <c r="B17" s="2" t="n">
-        <v>44031</v>
+        <v>44032</v>
       </c>
       <c r="C17" t="n">
-        <v>159045</v>
+        <v>161673</v>
       </c>
       <c r="D17" t="n">
-        <v>4104</v>
+        <v>4154</v>
       </c>
       <c r="E17" t="n">
-        <v>4250</v>
+        <v>4308</v>
       </c>
       <c r="F17" t="n">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="G17" t="n">
         <v>4.64</v>
       </c>
       <c r="H17" t="n">
-        <v>10.73</v>
+        <v>10.68</v>
       </c>
       <c r="I17" t="b">
         <v>0</v>
@@ -1287,10 +1287,10 @@
         <v>0</v>
       </c>
       <c r="K17" t="n">
-        <v>91616</v>
+        <v>92881</v>
       </c>
       <c r="L17" t="n">
-        <v>3820</v>
+        <v>3867</v>
       </c>
       <c r="M17" t="n">
         <v>823987</v>
@@ -1362,25 +1362,25 @@
         </is>
       </c>
       <c r="B19" s="2" t="n">
-        <v>44031</v>
+        <v>44032</v>
       </c>
       <c r="C19" t="n">
-        <v>43889</v>
+        <v>45524</v>
       </c>
       <c r="D19" t="n">
-        <v>1358</v>
+        <v>1389</v>
       </c>
       <c r="E19" t="n">
-        <v>19896</v>
+        <v>20429</v>
       </c>
       <c r="F19" t="n">
-        <v>679</v>
+        <v>696</v>
       </c>
       <c r="G19" t="n">
-        <v>45.33</v>
+        <v>44.88</v>
       </c>
       <c r="H19" t="n">
-        <v>50</v>
+        <v>50.11</v>
       </c>
       <c r="I19" t="b">
         <v>1</v>
@@ -1409,25 +1409,25 @@
         </is>
       </c>
       <c r="B20" s="2" t="n">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="C20" t="n">
-        <v>145183</v>
+        <v>148683</v>
       </c>
       <c r="D20" t="n">
-        <v>2784</v>
+        <v>2918</v>
       </c>
       <c r="E20" t="n">
-        <v>3119</v>
+        <v>3207</v>
       </c>
       <c r="F20" t="n">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="G20" t="n">
-        <v>4.3</v>
+        <v>4.32</v>
       </c>
       <c r="H20" t="n">
-        <v>3.46</v>
+        <v>3.57</v>
       </c>
       <c r="I20" t="b">
         <v>0</v>
@@ -1436,10 +1436,10 @@
         <v>0</v>
       </c>
       <c r="K20" t="n">
-        <v>72540</v>
+        <v>74216</v>
       </c>
       <c r="L20" t="n">
-        <v>2344</v>
+        <v>2440</v>
       </c>
       <c r="M20" t="n">
         <v>305259</v>
@@ -1460,22 +1460,22 @@
         </is>
       </c>
       <c r="B21" s="2" t="n">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="C21" t="n">
-        <v>98872</v>
+        <v>99875</v>
       </c>
       <c r="D21" t="n">
-        <v>7018</v>
+        <v>7038</v>
       </c>
       <c r="E21" t="n">
-        <v>13860</v>
+        <v>13956</v>
       </c>
       <c r="F21" t="n">
         <v>1484</v>
       </c>
       <c r="G21" t="n">
-        <v>30.21</v>
+        <v>30.06</v>
       </c>
       <c r="H21" t="n">
         <v>21.22</v>
@@ -1487,7 +1487,7 @@
         <v>1</v>
       </c>
       <c r="K21" t="n">
-        <v>45885</v>
+        <v>46430</v>
       </c>
       <c r="L21" t="n">
         <v>6992</v>
@@ -1511,25 +1511,25 @@
         </is>
       </c>
       <c r="B22" s="2" t="n">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="C22" t="n">
-        <v>355899</v>
+        <v>365244</v>
       </c>
       <c r="D22" t="n">
-        <v>5072</v>
+        <v>5206</v>
       </c>
       <c r="E22" t="n">
-        <v>42912</v>
+        <v>43924</v>
       </c>
       <c r="F22" t="n">
-        <v>965</v>
+        <v>991</v>
       </c>
       <c r="G22" t="n">
-        <v>12.06</v>
+        <v>12.03</v>
       </c>
       <c r="H22" t="n">
-        <v>19.03</v>
+        <v>19.04</v>
       </c>
       <c r="I22" t="b">
         <v>1</v>
@@ -1558,20 +1558,20 @@
         </is>
       </c>
       <c r="B23" s="2" t="n">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="C23" t="n">
-        <v>2621</v>
+        <v>2712</v>
       </c>
       <c r="D23" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E23" t="n">
         <v>15</v>
       </c>
       <c r="F23" t="inlineStr"/>
       <c r="G23" t="n">
-        <v>0.57</v>
+        <v>0.55</v>
       </c>
       <c r="H23" t="inlineStr"/>
       <c r="I23" t="b">
@@ -1601,22 +1601,22 @@
         </is>
       </c>
       <c r="B24" s="2" t="n">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="C24" t="n">
-        <v>1360</v>
+        <v>1366</v>
       </c>
       <c r="D24" t="n">
         <v>56</v>
       </c>
       <c r="E24" t="n">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F24" t="n">
         <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>11.36</v>
+        <v>11.38</v>
       </c>
       <c r="H24" t="n">
         <v>0</v>
@@ -1628,7 +1628,7 @@
         <v>1</v>
       </c>
       <c r="K24" t="n">
-        <v>1321</v>
+        <v>1327</v>
       </c>
       <c r="L24" t="n">
         <v>56</v>
@@ -1652,25 +1652,25 @@
         </is>
       </c>
       <c r="B25" s="2" t="n">
-        <v>44031</v>
+        <v>44032</v>
       </c>
       <c r="C25" t="n">
-        <v>46071</v>
+        <v>46116</v>
       </c>
       <c r="D25" t="n">
-        <v>3525</v>
+        <v>3527</v>
       </c>
       <c r="E25" t="n">
-        <v>6292</v>
+        <v>6312</v>
       </c>
       <c r="F25" t="n">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="G25" t="n">
-        <v>13.66</v>
+        <v>13.69</v>
       </c>
       <c r="H25" t="n">
-        <v>18.52</v>
+        <v>18.49</v>
       </c>
       <c r="I25" t="b">
         <v>1</v>
@@ -1750,25 +1750,25 @@
         </is>
       </c>
       <c r="B27" s="2" t="n">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="C27" t="n">
-        <v>40566</v>
+        <v>41059</v>
       </c>
       <c r="D27" t="n">
-        <v>1758</v>
+        <v>1763</v>
       </c>
       <c r="E27" t="n">
-        <v>2004</v>
+        <v>2012</v>
       </c>
       <c r="F27" t="n">
         <v>118</v>
       </c>
       <c r="G27" t="n">
-        <v>6.22</v>
+        <v>6.19</v>
       </c>
       <c r="H27" t="n">
-        <v>6.94</v>
+        <v>6.92</v>
       </c>
       <c r="I27" t="b">
         <v>0</v>
@@ -1777,10 +1777,10 @@
         <v>0</v>
       </c>
       <c r="K27" t="n">
-        <v>32201</v>
+        <v>32519</v>
       </c>
       <c r="L27" t="n">
-        <v>1701</v>
+        <v>1706</v>
       </c>
       <c r="M27" t="n">
         <v>227938</v>
@@ -1801,25 +1801,25 @@
         </is>
       </c>
       <c r="B28" s="2" t="n">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="C28" t="n">
-        <v>22847</v>
+        <v>23190</v>
       </c>
       <c r="D28" t="n">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="E28" t="n">
-        <v>1352</v>
+        <v>1369</v>
       </c>
       <c r="F28" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G28" t="n">
-        <v>7.63</v>
+        <v>7.61</v>
       </c>
       <c r="H28" t="n">
-        <v>7.64</v>
+        <v>7.67</v>
       </c>
       <c r="I28" t="b">
         <v>0</v>
@@ -1828,10 +1828,10 @@
         <v>1</v>
       </c>
       <c r="K28" t="n">
-        <v>17730</v>
+        <v>17993</v>
       </c>
       <c r="L28" t="n">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="M28" t="n">
         <v>90860</v>
@@ -1852,25 +1852,25 @@
         </is>
       </c>
       <c r="B29" s="2" t="n">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="C29" t="n">
-        <v>74068</v>
+        <v>74637</v>
       </c>
       <c r="D29" t="n">
-        <v>6047</v>
+        <v>6051</v>
       </c>
       <c r="E29" t="n">
-        <v>21359</v>
+        <v>21478</v>
       </c>
       <c r="F29" t="n">
-        <v>2407</v>
+        <v>2411</v>
       </c>
       <c r="G29" t="n">
-        <v>28.84</v>
+        <v>28.78</v>
       </c>
       <c r="H29" t="n">
-        <v>39.8</v>
+        <v>39.84</v>
       </c>
       <c r="I29" t="b">
         <v>1</v>
@@ -1902,10 +1902,10 @@
         <v>44027</v>
       </c>
       <c r="C30" t="n">
-        <v>94892</v>
+        <v>96583</v>
       </c>
       <c r="D30" t="n">
-        <v>3462</v>
+        <v>3498</v>
       </c>
       <c r="E30" t="n">
         <v>32137</v>
@@ -1950,25 +1950,25 @@
         </is>
       </c>
       <c r="B31" s="3" t="n">
-        <v>44031</v>
+        <v>44032</v>
       </c>
       <c r="C31" t="n">
-        <v>391538</v>
+        <v>400769</v>
       </c>
       <c r="D31" t="n">
-        <v>7694</v>
+        <v>7755</v>
       </c>
       <c r="E31" t="n">
-        <v>10866</v>
+        <v>11069</v>
       </c>
       <c r="F31" t="n">
         <v>654</v>
       </c>
       <c r="G31" t="n">
-        <v>4.32</v>
+        <v>4.3</v>
       </c>
       <c r="H31" t="n">
-        <v>8.69</v>
+        <v>8.66</v>
       </c>
       <c r="I31" t="b">
         <v>0</v>
@@ -1977,10 +1977,10 @@
         <v>0</v>
       </c>
       <c r="K31" t="n">
-        <v>251660</v>
+        <v>257550</v>
       </c>
       <c r="L31" t="n">
-        <v>7530</v>
+        <v>7555</v>
       </c>
       <c r="M31" t="n">
         <v>2267875</v>
@@ -2001,25 +2001,25 @@
         </is>
       </c>
       <c r="B32" s="2" t="n">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="C32" t="n">
-        <v>57206</v>
+        <v>57916</v>
       </c>
       <c r="D32" t="n">
-        <v>2632</v>
+        <v>2652</v>
       </c>
       <c r="E32" t="n">
-        <v>6611</v>
+        <v>6651</v>
       </c>
       <c r="F32" t="n">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="G32" t="n">
-        <v>11.56</v>
+        <v>11.48</v>
       </c>
       <c r="H32" t="n">
-        <v>14.17</v>
+        <v>14.14</v>
       </c>
       <c r="I32" t="b">
         <v>1</v>
@@ -2048,22 +2048,22 @@
         </is>
       </c>
       <c r="B33" s="2" t="n">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="C33" t="n">
-        <v>1949</v>
+        <v>2041</v>
       </c>
       <c r="D33" t="n">
         <v>18</v>
       </c>
       <c r="E33" t="n">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F33" t="n">
         <v>0</v>
       </c>
       <c r="G33" t="n">
-        <v>3.76</v>
+        <v>3.73</v>
       </c>
       <c r="H33" t="n">
         <v>0</v>
@@ -2075,7 +2075,7 @@
         <v>1</v>
       </c>
       <c r="K33" t="n">
-        <v>1251</v>
+        <v>1287</v>
       </c>
       <c r="L33" t="n">
         <v>18</v>
@@ -2098,21 +2098,39 @@
           <t>Wisconsin</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr"/>
-      <c r="C34" t="inlineStr"/>
-      <c r="D34" t="inlineStr"/>
-      <c r="E34" t="inlineStr"/>
-      <c r="F34" t="inlineStr"/>
-      <c r="G34" t="inlineStr"/>
-      <c r="H34" t="inlineStr"/>
+      <c r="B34" s="2" t="n">
+        <v>44033</v>
+      </c>
+      <c r="C34" t="n">
+        <v>44135</v>
+      </c>
+      <c r="D34" t="n">
+        <v>859</v>
+      </c>
+      <c r="E34" t="n">
+        <v>7019</v>
+      </c>
+      <c r="F34" t="n">
+        <v>196</v>
+      </c>
+      <c r="G34" t="n">
+        <v>17.59</v>
+      </c>
+      <c r="H34" t="n">
+        <v>23.2</v>
+      </c>
       <c r="I34" t="b">
         <v>0</v>
       </c>
       <c r="J34" t="b">
-        <v>0</v>
-      </c>
-      <c r="K34" t="inlineStr"/>
-      <c r="L34" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K34" t="n">
+        <v>39895</v>
+      </c>
+      <c r="L34" t="n">
+        <v>845</v>
+      </c>
       <c r="M34" t="n">
         <v>368744</v>
       </c>
@@ -2121,7 +2139,7 @@
       </c>
       <c r="O34" t="inlineStr">
         <is>
-          <t>An error occurred. ... Exception('Cannot perform query. Invalid query parameters.\nUnable to perform query. Please check your parameters.\n(Error Code: 400)')</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
@@ -2132,25 +2150,25 @@
         </is>
       </c>
       <c r="B35" s="2" t="n">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="C35" t="n">
-        <v>145575</v>
+        <v>148988</v>
       </c>
       <c r="D35" t="n">
-        <v>3176</v>
+        <v>3254</v>
       </c>
       <c r="E35" t="n">
-        <v>37250</v>
+        <v>38168</v>
       </c>
       <c r="F35" t="n">
-        <v>1473</v>
+        <v>1497</v>
       </c>
       <c r="G35" t="n">
-        <v>25.59</v>
+        <v>25.62</v>
       </c>
       <c r="H35" t="n">
-        <v>46.38</v>
+        <v>46</v>
       </c>
       <c r="I35" t="b">
         <v>1</v>
@@ -2179,16 +2197,16 @@
         </is>
       </c>
       <c r="B36" s="2" t="n">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="C36" t="n">
-        <v>47743</v>
+        <v>48575</v>
       </c>
       <c r="D36" t="n">
-        <v>1453</v>
+        <v>1465</v>
       </c>
       <c r="E36" t="n">
-        <v>1715</v>
+        <v>1732</v>
       </c>
       <c r="F36" t="n">
         <v>48</v>
@@ -2197,7 +2215,7 @@
         <v>5.44</v>
       </c>
       <c r="H36" t="n">
-        <v>3.45</v>
+        <v>3.42</v>
       </c>
       <c r="I36" t="b">
         <v>0</v>
@@ -2206,10 +2224,10 @@
         <v>0</v>
       </c>
       <c r="K36" t="n">
-        <v>31547</v>
+        <v>31843</v>
       </c>
       <c r="L36" t="n">
-        <v>1391</v>
+        <v>1403</v>
       </c>
       <c r="M36" t="n">
         <v>269854</v>
@@ -2230,13 +2248,13 @@
         </is>
       </c>
       <c r="B37" s="2" t="n">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="C37" t="n">
-        <v>6249</v>
+        <v>6262</v>
       </c>
       <c r="D37" t="n">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="E37" t="n">
         <v>321</v>
@@ -2245,10 +2263,10 @@
         <v>9</v>
       </c>
       <c r="G37" t="n">
-        <v>6.03</v>
+        <v>6</v>
       </c>
       <c r="H37" t="n">
-        <v>2.27</v>
+        <v>2.26</v>
       </c>
       <c r="I37" t="b">
         <v>0</v>
@@ -2257,10 +2275,10 @@
         <v>0</v>
       </c>
       <c r="K37" t="n">
-        <v>5326</v>
+        <v>5349</v>
       </c>
       <c r="L37" t="n">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="M37" t="n">
         <v>20516</v>
@@ -2280,18 +2298,32 @@
           <t>Washington, DC</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr"/>
-      <c r="C38" t="inlineStr"/>
-      <c r="D38" t="inlineStr"/>
-      <c r="E38" t="inlineStr"/>
-      <c r="F38" t="inlineStr"/>
-      <c r="G38" t="inlineStr"/>
-      <c r="H38" t="inlineStr"/>
+      <c r="B38" s="2" t="n">
+        <v>44033</v>
+      </c>
+      <c r="C38" t="n">
+        <v>1142</v>
+      </c>
+      <c r="D38" t="n">
+        <v>580</v>
+      </c>
+      <c r="E38" t="n">
+        <v>5591</v>
+      </c>
+      <c r="F38" t="n">
+        <v>428</v>
+      </c>
+      <c r="G38" t="n">
+        <v>489.58</v>
+      </c>
+      <c r="H38" t="n">
+        <v>73.79000000000001</v>
+      </c>
       <c r="I38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J38" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K38" t="inlineStr"/>
       <c r="L38" t="inlineStr"/>
@@ -2303,7 +2335,7 @@
       </c>
       <c r="O38" t="inlineStr">
         <is>
-          <t>An error occurred. ... HTTPError('404 Client Error: Not Found for url: https://coronavirus.dc.gov/sites/default/files/dc/sites/coronavirus/page_content/attachments/DC-COVID-19-Data-for-July-20-2020.xlsx')</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
@@ -2313,29 +2345,15 @@
           <t>Delaware</t>
         </is>
       </c>
-      <c r="B39" s="2" t="n">
-        <v>44032</v>
-      </c>
-      <c r="C39" t="n">
-        <v>13624</v>
-      </c>
-      <c r="D39" t="n">
-        <v>523</v>
-      </c>
-      <c r="E39" t="n">
-        <v>3478</v>
-      </c>
-      <c r="F39" t="n">
-        <v>134</v>
-      </c>
-      <c r="G39" t="n">
-        <v>25.53</v>
-      </c>
-      <c r="H39" t="n">
-        <v>25.62</v>
-      </c>
+      <c r="B39" t="inlineStr"/>
+      <c r="C39" t="inlineStr"/>
+      <c r="D39" t="inlineStr"/>
+      <c r="E39" t="inlineStr"/>
+      <c r="F39" t="inlineStr"/>
+      <c r="G39" t="inlineStr"/>
+      <c r="H39" t="inlineStr"/>
       <c r="I39" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J39" t="b">
         <v>0</v>
@@ -2350,7 +2368,7 @@
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... HTTPError('504 Server Error: Gateway Time-out for url: https://myhealthycommunity.dhss.delaware.gov/locations/state/')</t>
         </is>
       </c>
     </row>
@@ -2409,13 +2427,13 @@
         <v>44033</v>
       </c>
       <c r="C41" t="n">
-        <v>39419</v>
+        <v>39558</v>
       </c>
       <c r="D41" t="n">
-        <v>798</v>
+        <v>803</v>
       </c>
       <c r="E41" t="n">
-        <v>3239</v>
+        <v>3252</v>
       </c>
       <c r="F41" t="n">
         <v>38</v>
@@ -2424,7 +2442,7 @@
         <v>8.220000000000001</v>
       </c>
       <c r="H41" t="n">
-        <v>4.76</v>
+        <v>4.73</v>
       </c>
       <c r="I41" t="b">
         <v>1</v>
@@ -2453,25 +2471,25 @@
         </is>
       </c>
       <c r="B42" s="2" t="n">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="C42" t="n">
-        <v>101046</v>
+        <v>102861</v>
       </c>
       <c r="D42" t="n">
-        <v>1642</v>
+        <v>1668</v>
       </c>
       <c r="E42" t="n">
-        <v>16378</v>
+        <v>16812</v>
       </c>
       <c r="F42" t="n">
-        <v>520</v>
+        <v>530</v>
       </c>
       <c r="G42" t="n">
-        <v>23.93</v>
+        <v>23.98</v>
       </c>
       <c r="H42" t="n">
-        <v>32.79</v>
+        <v>32.9</v>
       </c>
       <c r="I42" t="b">
         <v>0</v>
@@ -2480,10 +2498,10 @@
         <v>1</v>
       </c>
       <c r="K42" t="n">
-        <v>68454</v>
+        <v>70100</v>
       </c>
       <c r="L42" t="n">
-        <v>1586</v>
+        <v>1611</v>
       </c>
       <c r="M42" t="n">
         <v>2179622</v>
@@ -2504,25 +2522,25 @@
         </is>
       </c>
       <c r="B43" s="2" t="n">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="C43" t="n">
-        <v>162748</v>
+        <v>163703</v>
       </c>
       <c r="D43" t="n">
-        <v>7301</v>
+        <v>7324</v>
       </c>
       <c r="E43" t="n">
-        <v>27337</v>
+        <v>27492</v>
       </c>
       <c r="F43" t="n">
-        <v>2014</v>
+        <v>2018</v>
       </c>
       <c r="G43" t="n">
-        <v>16.8</v>
+        <v>16.79</v>
       </c>
       <c r="H43" t="n">
-        <v>27.59</v>
+        <v>27.55</v>
       </c>
       <c r="I43" t="b">
         <v>1</v>
@@ -2551,25 +2569,25 @@
         </is>
       </c>
       <c r="B44" s="2" t="n">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="C44" t="n">
-        <v>15266</v>
+        <v>15822</v>
       </c>
       <c r="D44" t="n">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="E44" t="n">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="F44" t="n">
         <v>1</v>
       </c>
       <c r="G44" t="n">
-        <v>1.28</v>
+        <v>1.27</v>
       </c>
       <c r="H44" t="n">
-        <v>0.83</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="I44" t="b">
         <v>0</v>
@@ -2598,13 +2616,13 @@
         </is>
       </c>
       <c r="B45" s="2" t="n">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="C45" t="n">
-        <v>47107</v>
+        <v>47457</v>
       </c>
       <c r="D45" t="n">
-        <v>1545</v>
+        <v>1548</v>
       </c>
       <c r="E45" t="n">
         <v>9345</v>
@@ -2613,10 +2631,10 @@
         <v>151</v>
       </c>
       <c r="G45" t="n">
-        <v>19.84</v>
+        <v>19.69</v>
       </c>
       <c r="H45" t="n">
-        <v>9.77</v>
+        <v>9.75</v>
       </c>
       <c r="I45" t="b">
         <v>1</v>
@@ -2645,25 +2663,25 @@
         </is>
       </c>
       <c r="B46" s="2" t="n">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="C46" t="n">
-        <v>113789</v>
+        <v>114033</v>
       </c>
       <c r="D46" t="n">
-        <v>8433</v>
+        <v>8450</v>
       </c>
       <c r="E46" t="n">
-        <v>10674</v>
+        <v>10704</v>
       </c>
       <c r="F46" t="n">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="G46" t="n">
-        <v>9.380000000000001</v>
+        <v>9.390000000000001</v>
       </c>
       <c r="H46" t="n">
-        <v>8.19</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="I46" t="b">
         <v>1</v>
@@ -2692,22 +2710,22 @@
         </is>
       </c>
       <c r="B47" s="2" t="n">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="C47" t="n">
-        <v>16247</v>
+        <v>16555</v>
       </c>
       <c r="D47" t="n">
         <v>367</v>
       </c>
       <c r="E47" t="n">
-        <v>4636</v>
+        <v>4693</v>
       </c>
       <c r="F47" t="n">
         <v>146</v>
       </c>
       <c r="G47" t="n">
-        <v>30.83</v>
+        <v>30.57</v>
       </c>
       <c r="H47" t="n">
         <v>39.78</v>
@@ -2719,7 +2737,7 @@
         <v>0</v>
       </c>
       <c r="K47" t="n">
-        <v>15039</v>
+        <v>15354</v>
       </c>
       <c r="L47" t="n">
         <v>367</v>
@@ -2743,25 +2761,25 @@
         </is>
       </c>
       <c r="B48" s="2" t="n">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="C48" t="n">
-        <v>33621</v>
+        <v>34760</v>
       </c>
       <c r="D48" t="n">
-        <v>1132</v>
+        <v>1143</v>
       </c>
       <c r="E48" t="n">
-        <v>7793</v>
+        <v>7939</v>
       </c>
       <c r="F48" t="n">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="G48" t="n">
-        <v>32.37</v>
+        <v>31.99</v>
       </c>
       <c r="H48" t="n">
-        <v>35.92</v>
+        <v>36.06</v>
       </c>
       <c r="I48" t="b">
         <v>0</v>
@@ -2770,10 +2788,10 @@
         <v>1</v>
       </c>
       <c r="K48" t="n">
-        <v>24075</v>
+        <v>24820</v>
       </c>
       <c r="L48" t="n">
-        <v>1058</v>
+        <v>1065</v>
       </c>
       <c r="M48" t="n">
         <v>704896</v>

</xml_diff>

<commit_message>
Results from July 21, 2020 07:31:07 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-21.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-21.xlsx
@@ -2368,7 +2368,7 @@
       </c>
       <c r="O39" t="inlineStr">
         <is>
-          <t>An error occurred. ... HTTPError('504 Server Error: Gateway Time-out for url: https://myhealthycommunity.dhss.delaware.gov/locations/state/')</t>
+          <t>An error occurred. ... AttributeError("'numpy.float64' object has no attribute 'split'")</t>
         </is>
       </c>
     </row>
@@ -2427,13 +2427,13 @@
         <v>44033</v>
       </c>
       <c r="C41" t="n">
-        <v>39558</v>
+        <v>39582</v>
       </c>
       <c r="D41" t="n">
         <v>803</v>
       </c>
       <c r="E41" t="n">
-        <v>3252</v>
+        <v>3253</v>
       </c>
       <c r="F41" t="n">
         <v>38</v>

</xml_diff>